<commit_message>
Move to new CEDS working sectors. Add GAINS S content,  GAINS emf-30
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/CAN_scaling_mapping.xlsx
+++ b/input/mappings/scaling/CAN_scaling_mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="200" windowWidth="26620" windowHeight="18800" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14200" windowHeight="13320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="126">
   <si>
     <t>inv_sector</t>
   </si>
@@ -35,15 +35,9 @@
     <t>Abrasives Manufacture</t>
   </si>
   <si>
-    <t>industry</t>
-  </si>
-  <si>
     <t>Aluminum Industry</t>
   </si>
   <si>
-    <t>process_Al</t>
-  </si>
-  <si>
     <t>Asbestos Industry</t>
   </si>
   <si>
@@ -53,21 +47,12 @@
     <t>Bakeries</t>
   </si>
   <si>
-    <t>process_SAcidProduction</t>
-  </si>
-  <si>
     <t>Cement and Concrete Industry</t>
   </si>
   <si>
-    <t>industry_comb</t>
-  </si>
-  <si>
     <t>Chemicals Industry</t>
   </si>
   <si>
-    <t>industry_minerals</t>
-  </si>
-  <si>
     <t>Mineral Products Industry</t>
   </si>
   <si>
@@ -89,33 +74,18 @@
     <t>Non-Ferrous Smelting and Refining Industry</t>
   </si>
   <si>
-    <t>process_Smelting</t>
-  </si>
-  <si>
     <t>Pulp and Paper Industry</t>
   </si>
   <si>
-    <t>process_PulpPaper</t>
-  </si>
-  <si>
     <t>Wood Industry</t>
   </si>
   <si>
     <t>Upstream Petroleum Industry</t>
   </si>
   <si>
-    <t>oil_production</t>
-  </si>
-  <si>
     <t>Downstream Petroleum Industry</t>
   </si>
   <si>
-    <t>energytrans</t>
-  </si>
-  <si>
-    <t>energytrans_petr_refin</t>
-  </si>
-  <si>
     <t>Petroleum Product Transportation and Distribution</t>
   </si>
   <si>
@@ -125,15 +95,9 @@
     <t>Commercial Fuel Combustion</t>
   </si>
   <si>
-    <t>rescom_buildings</t>
-  </si>
-  <si>
     <t>Electric Power Generation (Utilities)</t>
   </si>
   <si>
-    <t>energytrans_electricity_gen</t>
-  </si>
-  <si>
     <t>Residential Fuel Combustion</t>
   </si>
   <si>
@@ -143,48 +107,24 @@
     <t>Air Transportation</t>
   </si>
   <si>
-    <t>transportation</t>
-  </si>
-  <si>
-    <t>transp_domestic_air</t>
-  </si>
-  <si>
     <t>Heavy-duty diesel vehicles</t>
   </si>
   <si>
-    <t>transp_domestic_ship</t>
-  </si>
-  <si>
     <t>Heavy-duty gasoline trucks</t>
   </si>
   <si>
-    <t>transp_road</t>
-  </si>
-  <si>
     <t>Light-duty diesel trucks</t>
   </si>
   <si>
-    <t>transp_rail</t>
-  </si>
-  <si>
     <t>Light-duty diesel vehicles</t>
   </si>
   <si>
-    <t>transp_unspecified</t>
-  </si>
-  <si>
     <t>Light-duty gasoline trucks</t>
   </si>
   <si>
-    <t>transp_international_ship</t>
-  </si>
-  <si>
     <t>Light-duty gasoline vehicles</t>
   </si>
   <si>
-    <t>transp_international_air</t>
-  </si>
-  <si>
     <t>Marine Transportation</t>
   </si>
   <si>
@@ -194,9 +134,6 @@
     <t>Off-road use of diesel</t>
   </si>
   <si>
-    <t>industry_agriculture</t>
-  </si>
-  <si>
     <t>Off-road use of gasoline/LPG/CNG</t>
   </si>
   <si>
@@ -212,36 +149,21 @@
     <t>Industrial &amp; Commercial Incineration</t>
   </si>
   <si>
-    <t>coal_production</t>
-  </si>
-  <si>
     <t>Municipal Incineration</t>
   </si>
   <si>
-    <t>natural_gas_production</t>
-  </si>
-  <si>
     <t>Other Incineration &amp; Utilities</t>
   </si>
   <si>
     <t>Cigarette Smoking</t>
   </si>
   <si>
-    <t>energytrans_heat_gen</t>
-  </si>
-  <si>
     <t>Dry Cleaning</t>
   </si>
   <si>
-    <t>energytrans_other</t>
-  </si>
-  <si>
     <t>General Solvent Use</t>
   </si>
   <si>
-    <t>energytrans_coke_ovens</t>
-  </si>
-  <si>
     <t>Marine Cargo Handling Industry</t>
   </si>
   <si>
@@ -251,15 +173,9 @@
     <t>Refined Petroleum Products Retail</t>
   </si>
   <si>
-    <t>unc_oil_production</t>
-  </si>
-  <si>
     <t>Printing</t>
   </si>
   <si>
-    <t>unc_gas_production</t>
-  </si>
-  <si>
     <t>Structural Fires</t>
   </si>
   <si>
@@ -272,9 +188,6 @@
     <t>Other Miscellaneous Sources</t>
   </si>
   <si>
-    <t>process_Other</t>
-  </si>
-  <si>
     <t>Agriculture</t>
   </si>
   <si>
@@ -326,17 +239,173 @@
     <t>NA</t>
   </si>
   <si>
-    <t>transp_air</t>
-  </si>
-  <si>
-    <t>petroleum</t>
+    <t>1A3b_Road</t>
+  </si>
+  <si>
+    <t>Road</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>1A3ai_International-aviation</t>
+  </si>
+  <si>
+    <t>1A3aii_Domestic-aviation</t>
+  </si>
+  <si>
+    <t>1A2b_Ind-Comb-Non-ferrous-metals</t>
+  </si>
+  <si>
+    <t>1A2c_Ind-Comb-Chemicals</t>
+  </si>
+  <si>
+    <t>Chemicals</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Pulp Paper</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Non-ferrous</t>
+  </si>
+  <si>
+    <t>Marine</t>
+  </si>
+  <si>
+    <t>Metals</t>
+  </si>
+  <si>
+    <t>Rail</t>
+  </si>
+  <si>
+    <t>2C_Metal-production</t>
+  </si>
+  <si>
+    <t>1A2a_Ind-Comb-Iron-steel</t>
+  </si>
+  <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>1A4a_Commercial-institutional</t>
+  </si>
+  <si>
+    <t>1A4b_Residential</t>
+  </si>
+  <si>
+    <t>1A1a_Electricity-public</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>Mining</t>
+  </si>
+  <si>
+    <t>1A2g_Ind-Comb-mining-quarying</t>
+  </si>
+  <si>
+    <t>5A_Solid-waste-disposal</t>
+  </si>
+  <si>
+    <t>5E_Other-waste-handling</t>
+  </si>
+  <si>
+    <t>5C_Waste-incineration</t>
+  </si>
+  <si>
+    <t>6A_Other-in-total</t>
+  </si>
+  <si>
+    <t>5D_Wastewater-handling</t>
+  </si>
+  <si>
+    <t>1A4c_Agriculture-forestry-fishing</t>
+  </si>
+  <si>
+    <t>Paint</t>
+  </si>
+  <si>
+    <t>2D_Paint-application</t>
+  </si>
+  <si>
+    <t>2D_Degreasing-Cleaning</t>
+  </si>
+  <si>
+    <t>3F_Agricultural-residue-burning-on-fields</t>
+  </si>
+  <si>
+    <t>3I_Agriculture-other</t>
+  </si>
+  <si>
+    <t>Ag-open</t>
+  </si>
+  <si>
+    <t>minerals</t>
+  </si>
+  <si>
+    <t>1A2f_Ind-Comb-Non-metalic-minerals</t>
+  </si>
+  <si>
+    <t>2A1_Cement-production</t>
+  </si>
+  <si>
+    <t>2A2_Lime-production</t>
+  </si>
+  <si>
+    <t>2A6_Other-minerals</t>
+  </si>
+  <si>
+    <t>other transformation</t>
+  </si>
+  <si>
+    <t>1A1bc_Other-transformation</t>
+  </si>
+  <si>
+    <t>Other_transformation</t>
+  </si>
+  <si>
+    <t>ag_open</t>
+  </si>
+  <si>
+    <t>ag_comb</t>
+  </si>
+  <si>
+    <t>other_transformation</t>
+  </si>
+  <si>
+    <t>2D3_Chemical-product-use</t>
+  </si>
+  <si>
+    <t>11B_Forest-fires</t>
+  </si>
+  <si>
+    <t>soil</t>
+  </si>
+  <si>
+    <t>3D_Soil-emissions</t>
+  </si>
+  <si>
+    <t>3D_Rice-Cultivation</t>
+  </si>
+  <si>
+    <t>3E_Enteric-fermentation</t>
+  </si>
+  <si>
+    <t>3B_Manure-management</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -367,11 +436,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -390,7 +454,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -444,13 +508,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -477,6 +574,23 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -503,6 +617,23 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -832,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -860,594 +991,651 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>92</v>
+      </c>
+      <c r="C23" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>73</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" t="s">
-        <v>57</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>46</v>
+      </c>
+      <c r="B45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>73</v>
-      </c>
-      <c r="B46" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>48</v>
+      </c>
+      <c r="B47" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>119</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>52</v>
+      </c>
+      <c r="B51" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>82</v>
-      </c>
-      <c r="C53" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>85</v>
-      </c>
-      <c r="B55" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>88</v>
+        <v>59</v>
+      </c>
+      <c r="B58" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>90</v>
+        <v>61</v>
+      </c>
+      <c r="B60" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>92</v>
+        <v>63</v>
+      </c>
+      <c r="B62" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>93</v>
+        <v>64</v>
+      </c>
+      <c r="B63" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="B64" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="C64" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="2:3">
       <c r="B65" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="C65" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="2:3">
       <c r="B66" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="C66" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="2:3">
       <c r="B67" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="C67" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="2:3">
       <c r="B68" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="C68" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="2:3">
       <c r="B69" t="s">
-        <v>101</v>
-      </c>
-      <c r="C69" t="s">
-        <v>53</v>
+        <v>94</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="2:3">
       <c r="B70" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="C70" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="2:3">
+      <c r="B71" t="s">
+        <v>59</v>
+      </c>
       <c r="C71" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
     </row>
     <row r="72" spans="2:3">
+      <c r="B72" t="s">
+        <v>59</v>
+      </c>
       <c r="C72" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
     </row>
     <row r="73" spans="2:3">
       <c r="B73" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="C73" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
     </row>
     <row r="74" spans="2:3">
       <c r="B74" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="C74" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="2:3">
+      <c r="B75" t="s">
+        <v>59</v>
+      </c>
       <c r="C75" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
     </row>
     <row r="76" spans="2:3">
       <c r="B76" t="s">
-        <v>29</v>
+        <v>116</v>
       </c>
       <c r="C76" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
     </row>
     <row r="77" spans="2:3">
       <c r="B77" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="C77" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
     </row>
     <row r="78" spans="2:3">
+      <c r="B78" t="s">
+        <v>116</v>
+      </c>
       <c r="C78" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" spans="2:3">
       <c r="B79" t="s">
-        <v>102</v>
-      </c>
-      <c r="C79" t="s">
-        <v>30</v>
+        <v>108</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="80" spans="2:3">
-      <c r="B80" t="s">
-        <v>102</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="C80" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3">
+      <c r="C81" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3">
+      <c r="C82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3">
+      <c r="B83" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C84" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3">
+      <c r="B85" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C85" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3">
+      <c r="B86" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C86" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3">
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="2:3">
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="2:3">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="2:3">
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="2:3">
+      <c r="B91" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1477,36 +1665,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1524,7 +1712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
@@ -1532,30 +1720,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update base SO2 EF for biomass and natural gas (still needs tweaking). Updated CAN and US scaling mapping files
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/CAN_scaling_mapping.xlsx
+++ b/input/mappings/scaling/CAN_scaling_mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14200" windowHeight="13320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22020" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="158">
   <si>
     <t>inv_sector</t>
   </si>
@@ -260,21 +260,6 @@
     <t>1A2c_Ind-Comb-Chemicals</t>
   </si>
   <si>
-    <t>Chemicals</t>
-  </si>
-  <si>
-    <t>Food</t>
-  </si>
-  <si>
-    <t>Pulp Paper</t>
-  </si>
-  <si>
-    <t>Wood</t>
-  </si>
-  <si>
-    <t>Non-ferrous</t>
-  </si>
-  <si>
     <t>Marine</t>
   </si>
   <si>
@@ -344,9 +329,6 @@
     <t>3I_Agriculture-other</t>
   </si>
   <si>
-    <t>Ag-open</t>
-  </si>
-  <si>
     <t>minerals</t>
   </si>
   <si>
@@ -362,33 +344,15 @@
     <t>2A6_Other-minerals</t>
   </si>
   <si>
-    <t>other transformation</t>
-  </si>
-  <si>
     <t>1A1bc_Other-transformation</t>
   </si>
   <si>
-    <t>Other_transformation</t>
-  </si>
-  <si>
-    <t>ag_open</t>
-  </si>
-  <si>
-    <t>ag_comb</t>
-  </si>
-  <si>
-    <t>other_transformation</t>
-  </si>
-  <si>
     <t>2D3_Chemical-product-use</t>
   </si>
   <si>
     <t>11B_Forest-fires</t>
   </si>
   <si>
-    <t>soil</t>
-  </si>
-  <si>
     <t>3D_Soil-emissions</t>
   </si>
   <si>
@@ -399,6 +363,138 @@
   </si>
   <si>
     <t>3B_Manure-management</t>
+  </si>
+  <si>
+    <t>1A1a_Electricity-autoproducer</t>
+  </si>
+  <si>
+    <t>1A1a_Heat-production</t>
+  </si>
+  <si>
+    <t>1A2d_Ind-Comb-Pulp-paper</t>
+  </si>
+  <si>
+    <t>1A2e_Ind-Comb-Food-tobacco</t>
+  </si>
+  <si>
+    <t>1A2g_Ind-Comb-Construction</t>
+  </si>
+  <si>
+    <t>1A2g_Ind-Comb-machinery</t>
+  </si>
+  <si>
+    <t>1A2g_Ind-Comb-other</t>
+  </si>
+  <si>
+    <t>1A2g_Ind-Comb-textile-leather</t>
+  </si>
+  <si>
+    <t>1A2g_Ind-Comb-transpequip</t>
+  </si>
+  <si>
+    <t>1A2g_Ind-Comb-wood-products</t>
+  </si>
+  <si>
+    <t>1A3c_Rail</t>
+  </si>
+  <si>
+    <t>1A3di_International-shipping</t>
+  </si>
+  <si>
+    <t>1A3dii_Domestic-naviation</t>
+  </si>
+  <si>
+    <t>1A3eii_Other-transp</t>
+  </si>
+  <si>
+    <t>1A5_Other-unspecified</t>
+  </si>
+  <si>
+    <t>1B1_Fugitive-solid-fuels</t>
+  </si>
+  <si>
+    <t>1B2_Fugitive-petr-and-gas</t>
+  </si>
+  <si>
+    <t>1B2d_Fugitive-other-energy</t>
+  </si>
+  <si>
+    <t>2B_Chemical-industry</t>
+  </si>
+  <si>
+    <t>2D3_Other-product-use</t>
+  </si>
+  <si>
+    <t>2H_Pulp-and-paper-food-beverage-wood</t>
+  </si>
+  <si>
+    <t>2L_Other-process-emissions</t>
+  </si>
+  <si>
+    <t>6B_Other-not-in-total</t>
+  </si>
+  <si>
+    <t>7A_Fossil-fuel-fires</t>
+  </si>
+  <si>
+    <t>11A_Volcanoes</t>
+  </si>
+  <si>
+    <t>11C_Other-natural</t>
+  </si>
+  <si>
+    <t>Pulp-Paper-Wood</t>
+  </si>
+  <si>
+    <t>other-transformation</t>
+  </si>
+  <si>
+    <t>1A1a-Electricity-public</t>
+  </si>
+  <si>
+    <t>6A-Other-in-total</t>
+  </si>
+  <si>
+    <t>2D-Degreasing-Cleaning</t>
+  </si>
+  <si>
+    <t>2D3-Chemical-product-use</t>
+  </si>
+  <si>
+    <t>Other-Waste</t>
+  </si>
+  <si>
+    <t>off-road</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Need to check if this is included, likely not</t>
+  </si>
+  <si>
+    <t>Does this include Ag waste on fields?</t>
+  </si>
+  <si>
+    <t>Chemical-Industry</t>
+  </si>
+  <si>
+    <t>Other-Industrial</t>
+  </si>
+  <si>
+    <t>2D3-Other-product-use</t>
+  </si>
+  <si>
+    <t>1A3eii-Other-transp</t>
+  </si>
+  <si>
+    <t>5C-Waste-incineration</t>
+  </si>
+  <si>
+    <t>Dust from Coal Mining</t>
+  </si>
+  <si>
+    <t>Construction Operation</t>
   </si>
 </sst>
 </file>
@@ -437,12 +533,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -454,7 +556,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="329">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -542,12 +644,255 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="329">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -591,6 +936,127 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -634,6 +1100,127 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -963,10 +1550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -976,7 +1563,7 @@
     <col min="3" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -986,658 +1573,924 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="B5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+    <row r="12" spans="1:4">
+      <c r="B12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+      <c r="B13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+      <c r="B14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+      <c r="B15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>81</v>
-      </c>
-    </row>
     <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>113</v>
+        <v>80</v>
+      </c>
+      <c r="C20" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>140</v>
+      </c>
+      <c r="C24" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>141</v>
+      </c>
+      <c r="C26" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>141</v>
+      </c>
+      <c r="C28" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>141</v>
+      </c>
+      <c r="C29" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>31</v>
-      </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>141</v>
+      </c>
+      <c r="C30" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>73</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
         <v>33</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B43" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
         <v>34</v>
       </c>
-      <c r="B33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+      <c r="B44" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
         <v>35</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B45" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
         <v>36</v>
       </c>
-      <c r="B35" t="s">
-        <v>117</v>
-      </c>
-      <c r="C35" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+      <c r="B46" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
         <v>37</v>
       </c>
-      <c r="B36" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>45</v>
-      </c>
-      <c r="B44" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" t="s">
-        <v>104</v>
-      </c>
-      <c r="C45" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>48</v>
-      </c>
       <c r="B47" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>49</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="1:4">
       <c r="B48" t="s">
-        <v>113</v>
+        <v>147</v>
+      </c>
+      <c r="C48" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>119</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>119</v>
+        <v>81</v>
+      </c>
+      <c r="C49" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>39</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>155</v>
       </c>
       <c r="C51" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>41</v>
+      </c>
+      <c r="B52" t="s">
+        <v>155</v>
+      </c>
+      <c r="C52" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>42</v>
+      </c>
+      <c r="B53" t="s">
+        <v>155</v>
+      </c>
+      <c r="C53" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>155</v>
+      </c>
+      <c r="C54" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>44</v>
+      </c>
+      <c r="B55" t="s">
+        <v>143</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>45</v>
+      </c>
+      <c r="B56" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>46</v>
+      </c>
+      <c r="B57" t="s">
+        <v>144</v>
+      </c>
+      <c r="C57" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>143</v>
+      </c>
+      <c r="C58" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>48</v>
+      </c>
+      <c r="B59" t="s">
+        <v>143</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B60" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>50</v>
+      </c>
+      <c r="B61" t="s">
+        <v>145</v>
+      </c>
+      <c r="C61" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B62" t="s">
-        <v>121</v>
+        <v>143</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
+        <v>52</v>
+      </c>
+      <c r="B63" t="s">
+        <v>97</v>
+      </c>
+      <c r="C63" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>53</v>
+      </c>
+      <c r="B64" t="s">
+        <v>143</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>54</v>
+      </c>
+      <c r="B65" t="s">
+        <v>143</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>55</v>
+      </c>
+      <c r="B66" t="s">
+        <v>55</v>
+      </c>
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>56</v>
+      </c>
+      <c r="B67" t="s">
+        <v>147</v>
+      </c>
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>157</v>
+      </c>
+      <c r="B68" t="s">
+        <v>147</v>
+      </c>
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>57</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C69" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C70" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>156</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C71" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>59</v>
+      </c>
+      <c r="B72" t="s">
+        <v>146</v>
+      </c>
+      <c r="C72" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>60</v>
+      </c>
+      <c r="B73" t="s">
+        <v>143</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>61</v>
+      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>62</v>
+      </c>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>63</v>
+      </c>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
         <v>64</v>
       </c>
-      <c r="B63" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="B64" t="s">
-        <v>74</v>
-      </c>
-      <c r="C64" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3">
-      <c r="B65" t="s">
-        <v>74</v>
-      </c>
-      <c r="C65" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3">
-      <c r="B66" t="s">
-        <v>85</v>
-      </c>
-      <c r="C66" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3">
-      <c r="B67" t="s">
-        <v>85</v>
-      </c>
-      <c r="C67" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3">
-      <c r="B68" t="s">
-        <v>85</v>
-      </c>
-      <c r="C68" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3">
-      <c r="B69" t="s">
-        <v>94</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3">
-      <c r="B70" t="s">
-        <v>59</v>
-      </c>
-      <c r="C70" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3">
-      <c r="B71" t="s">
-        <v>59</v>
-      </c>
-      <c r="C71" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3">
-      <c r="B72" t="s">
-        <v>59</v>
-      </c>
-      <c r="C72" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3">
-      <c r="B73" t="s">
-        <v>59</v>
-      </c>
-      <c r="C73" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3">
-      <c r="B74" t="s">
-        <v>59</v>
-      </c>
-      <c r="C74" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="75" spans="2:3">
-      <c r="B75" t="s">
-        <v>59</v>
-      </c>
-      <c r="C75" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="76" spans="2:3">
-      <c r="B76" t="s">
-        <v>116</v>
-      </c>
-      <c r="C76" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="77" spans="2:3">
-      <c r="B77" t="s">
-        <v>116</v>
-      </c>
-      <c r="C77" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="78" spans="2:3">
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" spans="1:4">
       <c r="B78" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="C78" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="79" spans="2:3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="B79" t="s">
-        <v>108</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="80" spans="2:3">
+        <v>55</v>
+      </c>
+      <c r="C79" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="B80" t="s">
+        <v>55</v>
+      </c>
       <c r="C80" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="81" spans="2:3">
+      <c r="B81" t="s">
+        <v>55</v>
+      </c>
       <c r="C81" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" spans="2:3">
+      <c r="B82" t="s">
+        <v>55</v>
+      </c>
       <c r="C82" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3">
-      <c r="B83" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84" t="s">
+        <v>152</v>
+      </c>
+      <c r="C84" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3">
+      <c r="B85" t="s">
+        <v>152</v>
+      </c>
+      <c r="C85" t="s">
         <v>115</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3">
-      <c r="B84" s="1" t="s">
+    </row>
+    <row r="86" spans="2:3">
+      <c r="B86" t="s">
+        <v>152</v>
+      </c>
+      <c r="C86" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3">
+      <c r="B87" t="s">
+        <v>152</v>
+      </c>
+      <c r="C87" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3">
+      <c r="B88" t="s">
+        <v>152</v>
+      </c>
+      <c r="C88" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3">
+      <c r="B89" t="s">
+        <v>152</v>
+      </c>
+      <c r="C89" t="s">
         <v>121</v>
       </c>
-      <c r="C84" t="s">
+    </row>
+    <row r="90" spans="2:3">
+      <c r="B90" t="s">
+        <v>152</v>
+      </c>
+      <c r="C90" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="85" spans="2:3">
-      <c r="B85" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C85" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3">
-      <c r="B86" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C86" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3">
-      <c r="B87" s="1"/>
-    </row>
-    <row r="88" spans="2:3">
-      <c r="B88" s="1"/>
-    </row>
-    <row r="89" spans="2:3">
-      <c r="B89" s="1"/>
-    </row>
-    <row r="90" spans="2:3">
-      <c r="B90" s="1"/>
     </row>
     <row r="91" spans="2:3">
       <c r="B91" s="1"/>
     </row>
+    <row r="92" spans="2:3">
+      <c r="B92" s="1"/>
+      <c r="C92" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3">
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="2:3">
+      <c r="B94" s="1"/>
+      <c r="C94" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3">
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="2:3">
+      <c r="B96" s="1"/>
+      <c r="C96" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3">
+      <c r="B97" s="1"/>
+      <c r="C97" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3">
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="2:3">
+      <c r="B99" s="1"/>
+      <c r="C99" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3">
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="2:3">
+      <c r="B101" s="1"/>
+      <c r="C101" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3">
+      <c r="C103" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3">
+      <c r="C104" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3">
+      <c r="C105" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3">
+      <c r="C106" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3">
+      <c r="C107" t="s">
+        <v>139</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="C84:C101">
+    <sortCondition ref="C84:C101"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Update to EDGAR 4.3-PEGASOS, updates to scaling mappings, update US trends (to 2014) and China inventory
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/CAN_scaling_mapping.xlsx
+++ b/input/mappings/scaling/CAN_scaling_mapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22020" windowHeight="15480" tabRatio="500"/>
@@ -347,9 +347,6 @@
     <t>1A1bc_Other-transformation</t>
   </si>
   <si>
-    <t>2D3_Chemical-product-use</t>
-  </si>
-  <si>
     <t>11B_Forest-fires</t>
   </si>
   <si>
@@ -495,6 +492,9 @@
   </si>
   <si>
     <t>Construction Operation</t>
+  </si>
+  <si>
+    <t>2D3_Chemical-products-manufacture-processing</t>
   </si>
 </sst>
 </file>
@@ -1553,7 +1553,7 @@
   <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1574,7 +1574,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1582,7 +1582,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1598,7 +1598,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1606,10 +1606,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1617,7 +1617,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1660,7 +1660,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>78</v>
@@ -1668,10 +1668,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1687,7 +1687,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C14" t="s">
         <v>107</v>
@@ -1698,7 +1698,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1755,18 +1755,18 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="B22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1774,18 +1774,18 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="B24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1793,7 +1793,7 @@
         <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C25" t="s">
         <v>107</v>
@@ -1804,7 +1804,7 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C26" t="s">
         <v>107</v>
@@ -1815,7 +1815,7 @@
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C27" t="s">
         <v>107</v>
@@ -1823,26 +1823,26 @@
     </row>
     <row r="28" spans="1:3">
       <c r="B28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="B29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1850,7 +1850,7 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1869,7 +1869,7 @@
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C33" t="s">
         <v>87</v>
@@ -1906,7 +1906,7 @@
         <v>75</v>
       </c>
       <c r="D36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1981,7 +1981,7 @@
         <v>79</v>
       </c>
       <c r="C44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1998,7 +1998,7 @@
         <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C46" t="s">
         <v>96</v>
@@ -2009,16 +2009,16 @@
         <v>37</v>
       </c>
       <c r="B47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C47" s="2"/>
     </row>
     <row r="48" spans="1:4">
       <c r="B48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2029,7 +2029,7 @@
         <v>81</v>
       </c>
       <c r="C49" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2037,10 +2037,10 @@
         <v>39</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2048,7 +2048,7 @@
         <v>40</v>
       </c>
       <c r="B51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C51" t="s">
         <v>93</v>
@@ -2059,7 +2059,7 @@
         <v>41</v>
       </c>
       <c r="B52" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C52" t="s">
         <v>93</v>
@@ -2070,7 +2070,7 @@
         <v>42</v>
       </c>
       <c r="B53" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C53" t="s">
         <v>93</v>
@@ -2081,7 +2081,7 @@
         <v>43</v>
       </c>
       <c r="B54" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C54" t="s">
         <v>93</v>
@@ -2092,7 +2092,7 @@
         <v>44</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>94</v>
@@ -2103,7 +2103,7 @@
         <v>45</v>
       </c>
       <c r="B56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2111,7 +2111,7 @@
         <v>46</v>
       </c>
       <c r="B57" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C57" t="s">
         <v>99</v>
@@ -2122,7 +2122,7 @@
         <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C58" t="s">
         <v>94</v>
@@ -2133,7 +2133,7 @@
         <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>94</v>
@@ -2144,7 +2144,7 @@
         <v>49</v>
       </c>
       <c r="B60" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2152,10 +2152,10 @@
         <v>50</v>
       </c>
       <c r="B61" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C61" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2163,7 +2163,7 @@
         <v>51</v>
       </c>
       <c r="B62" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>94</v>
@@ -2185,7 +2185,7 @@
         <v>53</v>
       </c>
       <c r="B64" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>94</v>
@@ -2196,7 +2196,7 @@
         <v>54</v>
       </c>
       <c r="B65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>94</v>
@@ -2216,16 +2216,16 @@
         <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B68" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C68" s="1"/>
     </row>
@@ -2234,10 +2234,10 @@
         <v>57</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C69" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2245,21 +2245,21 @@
         <v>58</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C70" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C71" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2267,7 +2267,7 @@
         <v>59</v>
       </c>
       <c r="B72" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C72" t="s">
         <v>92</v>
@@ -2278,7 +2278,7 @@
         <v>60</v>
       </c>
       <c r="B73" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>94</v>
@@ -2291,7 +2291,7 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2320,7 +2320,7 @@
         <v>55</v>
       </c>
       <c r="C78" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2328,7 +2328,7 @@
         <v>55</v>
       </c>
       <c r="C79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2336,7 +2336,7 @@
         <v>55</v>
       </c>
       <c r="C80" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="2:3">
@@ -2344,7 +2344,7 @@
         <v>55</v>
       </c>
       <c r="C81" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="82" spans="2:3">
@@ -2357,58 +2357,58 @@
     </row>
     <row r="84" spans="2:3">
       <c r="B84" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C84" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="85" spans="2:3">
       <c r="B85" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C85" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="2:3">
       <c r="B86" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C86" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="2:3">
       <c r="B87" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C87" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" spans="2:3">
       <c r="B88" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C88" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="89" spans="2:3">
       <c r="B89" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C89" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="90" spans="2:3">
       <c r="B90" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C90" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="91" spans="2:3">
@@ -2417,7 +2417,7 @@
     <row r="92" spans="2:3">
       <c r="B92" s="1"/>
       <c r="C92" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="93" spans="2:3">
@@ -2426,7 +2426,7 @@
     <row r="94" spans="2:3">
       <c r="B94" s="1"/>
       <c r="C94" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="95" spans="2:3">
@@ -2450,7 +2450,7 @@
     <row r="99" spans="2:3">
       <c r="B99" s="1"/>
       <c r="C99" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="100" spans="2:3">
@@ -2464,27 +2464,27 @@
     </row>
     <row r="103" spans="2:3">
       <c r="C103" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="104" spans="2:3">
       <c r="C104" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="105" spans="2:3">
       <c r="C105" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="106" spans="2:3">
       <c r="C106" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="107" spans="2:3">
       <c r="C107" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove duplicate CEDS sectors in Canada scaling mapping
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/CAN_scaling_mapping.xlsx
+++ b/input/mappings/scaling/CAN_scaling_mapping.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="157">
   <si>
     <t>inv_sector</t>
   </si>
@@ -399,9 +399,6 @@
   </si>
   <si>
     <t>1A3dii_Domestic-naviation</t>
-  </si>
-  <si>
-    <t>1A3eii_Other-transp</t>
   </si>
   <si>
     <t>1A5_Other-unspecified</t>
@@ -556,8 +553,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="329">
+  <cellStyleXfs count="335">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -892,7 +895,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="329">
+  <cellStyles count="335">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1057,6 +1060,9 @@
     <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1221,6 +1227,9 @@
     <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1552,8 +1561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1574,7 +1583,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1582,7 +1591,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1598,7 +1607,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1606,10 +1615,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1617,7 +1626,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1660,7 +1669,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>78</v>
@@ -1668,10 +1677,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1687,7 +1696,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C14" t="s">
         <v>107</v>
@@ -1698,7 +1707,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1755,7 +1764,7 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C21" t="s">
         <v>115</v>
@@ -1763,10 +1772,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="B22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1774,15 +1783,13 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>139</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3">
       <c r="B24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C24" t="s">
         <v>122</v>
@@ -1793,56 +1800,50 @@
         <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>140</v>
-      </c>
-      <c r="C25" t="s">
-        <v>107</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>140</v>
-      </c>
-      <c r="C26" t="s">
-        <v>107</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>140</v>
-      </c>
-      <c r="C27" t="s">
-        <v>107</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3">
       <c r="B28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="B29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1850,7 +1851,7 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1869,7 +1870,7 @@
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C33" t="s">
         <v>87</v>
@@ -1906,7 +1907,7 @@
         <v>75</v>
       </c>
       <c r="D36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1998,7 +1999,7 @@
         <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C46" t="s">
         <v>96</v>
@@ -2009,13 +2010,13 @@
         <v>37</v>
       </c>
       <c r="B47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C47" s="2"/>
     </row>
     <row r="48" spans="1:4">
       <c r="B48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C48" t="s">
         <v>117</v>
@@ -2037,10 +2038,7 @@
         <v>39</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C50" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2048,7 +2046,7 @@
         <v>40</v>
       </c>
       <c r="B51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C51" t="s">
         <v>93</v>
@@ -2059,40 +2057,34 @@
         <v>41</v>
       </c>
       <c r="B52" t="s">
-        <v>154</v>
-      </c>
-      <c r="C52" t="s">
-        <v>93</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="C52" s="2"/>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>42</v>
       </c>
       <c r="B53" t="s">
-        <v>154</v>
-      </c>
-      <c r="C53" t="s">
-        <v>93</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="C53" s="2"/>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>43</v>
       </c>
       <c r="B54" t="s">
-        <v>154</v>
-      </c>
-      <c r="C54" t="s">
-        <v>93</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="C54" s="2"/>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>44</v>
       </c>
       <c r="B55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>94</v>
@@ -2103,7 +2095,7 @@
         <v>45</v>
       </c>
       <c r="B56" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2111,7 +2103,7 @@
         <v>46</v>
       </c>
       <c r="B57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C57" t="s">
         <v>99</v>
@@ -2122,29 +2114,25 @@
         <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>142</v>
-      </c>
-      <c r="C58" t="s">
-        <v>94</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C58" s="2"/>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>142</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C59" s="2"/>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>49</v>
       </c>
       <c r="B60" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2152,10 +2140,10 @@
         <v>50</v>
       </c>
       <c r="B61" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C61" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2163,11 +2151,9 @@
         <v>51</v>
       </c>
       <c r="B62" t="s">
-        <v>142</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
@@ -2185,22 +2171,18 @@
         <v>53</v>
       </c>
       <c r="B64" t="s">
-        <v>142</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C64" s="2"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>54</v>
       </c>
       <c r="B65" t="s">
-        <v>142</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C65" s="2"/>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
@@ -2216,16 +2198,16 @@
         <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B68" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C68" s="1"/>
     </row>
@@ -2234,10 +2216,7 @@
         <v>57</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C69" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2245,21 +2224,15 @@
         <v>58</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C70" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C71" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2267,7 +2240,7 @@
         <v>59</v>
       </c>
       <c r="B72" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C72" t="s">
         <v>92</v>
@@ -2278,11 +2251,9 @@
         <v>60</v>
       </c>
       <c r="B73" t="s">
-        <v>142</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
@@ -2291,7 +2262,7 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2357,7 +2328,7 @@
     </row>
     <row r="84" spans="2:3">
       <c r="B84" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C84" t="s">
         <v>113</v>
@@ -2365,7 +2336,7 @@
     </row>
     <row r="85" spans="2:3">
       <c r="B85" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C85" t="s">
         <v>114</v>
@@ -2373,7 +2344,7 @@
     </row>
     <row r="86" spans="2:3">
       <c r="B86" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C86" t="s">
         <v>116</v>
@@ -2381,7 +2352,7 @@
     </row>
     <row r="87" spans="2:3">
       <c r="B87" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C87" t="s">
         <v>118</v>
@@ -2389,7 +2360,7 @@
     </row>
     <row r="88" spans="2:3">
       <c r="B88" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C88" t="s">
         <v>119</v>
@@ -2397,7 +2368,7 @@
     </row>
     <row r="89" spans="2:3">
       <c r="B89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C89" t="s">
         <v>120</v>
@@ -2405,7 +2376,7 @@
     </row>
     <row r="90" spans="2:3">
       <c r="B90" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C90" t="s">
         <v>121</v>
@@ -2426,7 +2397,7 @@
     <row r="94" spans="2:3">
       <c r="B94" s="1"/>
       <c r="C94" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="95" spans="2:3">
@@ -2450,7 +2421,7 @@
     <row r="99" spans="2:3">
       <c r="B99" s="1"/>
       <c r="C99" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="100" spans="2:3">
@@ -2464,17 +2435,17 @@
     </row>
     <row r="103" spans="2:3">
       <c r="C103" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="104" spans="2:3">
       <c r="C104" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="105" spans="2:3">
       <c r="C105" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="106" spans="2:3">
@@ -2484,7 +2455,7 @@
     </row>
     <row r="107" spans="2:3">
       <c r="C107" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>